<commit_message>
add portal report analysis, updated eSMR scripts with joined supplemental data, and add pauses to SMARTS script
</commit_message>
<xml_diff>
--- a/eSMR/esmr-data-dictionary-tool/eSMR_Data_Dictionary_Template.xlsx
+++ b/eSMR/esmr-data-dictionary-tool/eSMR_Data_Dictionary_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/CA_data_portal/Surface-Water-Datasets/esmr-data-dictionary-tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/CA_data_portal/eSMR/esmr-data-dictionary-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{30876149-88FF-4E97-8253-FCDDC3174AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{27818DA8-DBEF-4A06-AC73-B4BF7276930F}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{30876149-88FF-4E97-8253-FCDDC3174AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5488BF3B-3D2D-4033-9FCD-2FB1769B004F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
   <si>
     <t>column</t>
   </si>
@@ -356,6 +356,33 @@
 • &gt;=
 • ND (Non-detect)
 • DNQ (Detected but not Quantified)</t>
+  </si>
+  <si>
+    <t>wdid</t>
+  </si>
+  <si>
+    <t>npdes_num</t>
+  </si>
+  <si>
+    <t>design_flow</t>
+  </si>
+  <si>
+    <t>facility_place_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_place_city </t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_place_county </t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_place_zip </t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_place_latitude </t>
+  </si>
+  <si>
+    <t>facility_place_longitude</t>
   </si>
 </sst>
 </file>
@@ -1277,11 +1304,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,6 +1791,96 @@
         <v>73</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="5"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{B486371E-9CA5-461A-A7F9-634A8F7EA92C}">

</xml_diff>

<commit_message>
add new version of portal report, and wastewater enforcement actions update script
</commit_message>
<xml_diff>
--- a/eSMR/esmr-data-dictionary-tool/eSMR_Data_Dictionary_Template.xlsx
+++ b/eSMR/esmr-data-dictionary-tool/eSMR_Data_Dictionary_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/CA_data_portal/eSMR/esmr-data-dictionary-tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daltare\OneDrive - Water Boards\projects\CA_data_portal\eSMR\esmr-data-dictionary-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{30876149-88FF-4E97-8253-FCDDC3174AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5488BF3B-3D2D-4033-9FCD-2FB1769B004F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359E3236-029D-40CE-97EE-F7FA56B2F41E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eSMR_Data_Dictionary" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t>column</t>
   </si>
@@ -356,33 +356,6 @@
 • &gt;=
 • ND (Non-detect)
 • DNQ (Detected but not Quantified)</t>
-  </si>
-  <si>
-    <t>wdid</t>
-  </si>
-  <si>
-    <t>npdes_num</t>
-  </si>
-  <si>
-    <t>design_flow</t>
-  </si>
-  <si>
-    <t>facility_place_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_place_city </t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_place_county </t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_place_zip </t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_place_latitude </t>
-  </si>
-  <si>
-    <t>facility_place_longitude</t>
   </si>
 </sst>
 </file>
@@ -1304,24 +1277,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="103.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="103.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1310,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1353,7 +1326,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="276.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="252.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1369,7 +1342,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1385,7 +1358,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="180.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="180.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1401,7 +1374,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1390,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="84.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="84.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1433,7 +1406,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="84.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1449,7 +1422,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1465,7 +1438,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="180.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="180.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1454,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1497,7 +1470,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1513,7 +1486,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1529,7 +1502,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1545,7 +1518,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1561,7 +1534,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1577,7 +1550,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1593,7 +1566,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
@@ -1609,7 +1582,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
@@ -1625,7 +1598,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1641,7 +1614,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1657,7 +1630,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -1673,7 +1646,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
@@ -1689,7 +1662,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
@@ -1705,7 +1678,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
@@ -1721,7 +1694,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
@@ -1735,7 +1708,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>31</v>
       </c>
@@ -1749,7 +1722,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>32</v>
       </c>
@@ -1763,7 +1736,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
@@ -1777,7 +1750,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>34</v>
       </c>
@@ -1790,96 +1763,6 @@
       <c r="D30" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>